<commit_message>
changes incorporated based on Grigorii
</commit_message>
<xml_diff>
--- a/input_file.xlsx
+++ b/input_file.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NandhiniRamachandran\Documents\softwares\Windstream\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513E49FE-810F-4C61-8244-28B36B7318C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631DC87E-C2CE-465B-AC2A-66A452E47FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7344" yWindow="0" windowWidth="14904" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Input_config" sheetId="1" r:id="rId1"/>
+    <sheet name="input_config" sheetId="1" r:id="rId1"/>
     <sheet name="input_config_2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -384,7 +384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -509,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59326E29-94B9-4B73-A1C5-7783227550FF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>